<commit_message>
AMEND DATA IMPORT TEMPLATE [DELIVERY_HAITONG_N]
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/DataTemplate/Delivery/HaiTong_N.xlsx
+++ b/src/Presentation/CTM.Win/DataTemplate/Delivery/HaiTong_N.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>成交日期</t>
   </si>
@@ -37,75 +37,62 @@
     <t>成交金额</t>
   </si>
   <si>
-    <t>可用余额</t>
-  </si>
-  <si>
     <t>发生金额</t>
   </si>
   <si>
-    <t>手续费</t>
-  </si>
-  <si>
-    <t>印花税</t>
-  </si>
-  <si>
-    <t>其他杂费</t>
-  </si>
-  <si>
     <t>资金余额</t>
   </si>
   <si>
-    <t>合同编号</t>
-  </si>
-  <si>
     <t>股东帐户</t>
   </si>
   <si>
-    <t>过户费</t>
-  </si>
-  <si>
-    <t>交易币种</t>
-  </si>
-  <si>
-    <t>结算币种</t>
-  </si>
-  <si>
-    <t>结算汇率</t>
-  </si>
-  <si>
-    <t>港股交易费</t>
-  </si>
-  <si>
-    <t>帝王洁具</t>
-  </si>
-  <si>
     <t>买</t>
   </si>
   <si>
-    <t>人民币</t>
+    <t>流水号</t>
+  </si>
+  <si>
+    <t>摘要</t>
+  </si>
+  <si>
+    <t>成交编号</t>
+  </si>
+  <si>
+    <t>交易市场</t>
+  </si>
+  <si>
+    <t>港股通结算汇率</t>
+  </si>
+  <si>
+    <t>过户费￥/使用费HK$</t>
+  </si>
+  <si>
+    <t>印花税￥/港股印花税HK$</t>
+  </si>
+  <si>
+    <t>其他费用￥/港股其他费用HK$</t>
   </si>
   <si>
     <t>交易类别</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日内</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>波段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>目标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>证券买入:帝王洁具</t>
+  </si>
+  <si>
+    <t>波段</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +104,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -450,272 +444,335 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>20170124</v>
-      </c>
-      <c r="B2" s="1">
+        <v>20170512</v>
+      </c>
+      <c r="C2" s="1">
         <v>2798</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-144043.20000000001</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1868546.93</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="1">
+        <v>3000</v>
+      </c>
+      <c r="J2" s="1">
+        <v>48</v>
+      </c>
+      <c r="K2" s="1">
+        <v>144000</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10100000761</v>
+      </c>
+      <c r="N2" s="1">
+        <v>105073273</v>
+      </c>
+      <c r="O2" s="1">
+        <v>1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>20170512</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2798</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-120036</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1748510.93</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="1">
+        <v>2500</v>
+      </c>
+      <c r="J3" s="1">
+        <v>48</v>
+      </c>
+      <c r="K3" s="1">
+        <v>120000</v>
+      </c>
+      <c r="L3" s="1">
+        <v>10100000764</v>
+      </c>
+      <c r="N3" s="1">
+        <v>105073273</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>20170512</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2798</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-14405</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1734105.93</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="1">
+        <v>300</v>
+      </c>
+      <c r="J4" s="1">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1">
+        <v>14400</v>
+      </c>
+      <c r="L4" s="1">
+        <v>10100000764</v>
+      </c>
+      <c r="N4" s="1">
+        <v>105073273</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1">
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1">
+        <v>20170512</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2798</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-9605</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1724500.93</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="1">
+        <v>200</v>
+      </c>
+      <c r="J5" s="1">
+        <v>48</v>
+      </c>
+      <c r="K5" s="1">
+        <v>9600</v>
+      </c>
+      <c r="L5" s="1">
+        <v>10100000764</v>
+      </c>
+      <c r="N5" s="1">
+        <v>105073273</v>
+      </c>
+      <c r="O5" s="1">
+        <v>1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1">
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>20170512</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2798</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1">
+        <v>-4805</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1719695.93</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="1">
-        <v>800</v>
-      </c>
-      <c r="F2" s="1">
-        <v>50.899000000000001</v>
-      </c>
-      <c r="G2" s="1">
-        <v>40719</v>
-      </c>
-      <c r="H2" s="1">
-        <v>800</v>
-      </c>
-      <c r="I2" s="1">
-        <v>-40731.22</v>
-      </c>
-      <c r="J2" s="1">
-        <v>12.22</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-      <c r="M2" s="1">
-        <v>4064494.39</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3013</v>
-      </c>
-      <c r="O2" s="1">
-        <v>189845491</v>
-      </c>
-      <c r="P2" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+      <c r="J6" s="1">
+        <v>48</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4800</v>
+      </c>
+      <c r="L6" s="1">
+        <v>10100000765</v>
+      </c>
+      <c r="N6" s="1">
+        <v>105073273</v>
+      </c>
+      <c r="O6" s="1">
+        <v>1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>0</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="1">
-        <v>1</v>
-      </c>
-      <c r="T2" s="1">
-        <v>0</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
-        <v>20170124</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2798</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="1">
-        <v>600</v>
-      </c>
-      <c r="F3" s="1">
-        <v>50.84</v>
-      </c>
-      <c r="G3" s="1">
-        <v>30504</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1400</v>
-      </c>
-      <c r="I3" s="1">
-        <v>-30513.15</v>
-      </c>
-      <c r="J3" s="1">
-        <v>9.15</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>4033981.24</v>
-      </c>
-      <c r="N3" s="1">
-        <v>3011</v>
-      </c>
-      <c r="O3" s="1">
-        <v>189845491</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1">
-        <v>20170124</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2798</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="1">
-        <v>300</v>
-      </c>
-      <c r="F4" s="1">
-        <v>50.77</v>
-      </c>
-      <c r="G4" s="1">
-        <v>15231</v>
-      </c>
-      <c r="H4" s="1">
-        <v>1700</v>
-      </c>
-      <c r="I4" s="1">
-        <v>-15236</v>
-      </c>
-      <c r="J4" s="1">
-        <v>5</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>4018745.24</v>
-      </c>
-      <c r="N4" s="1">
-        <v>3020</v>
-      </c>
-      <c r="O4" s="1">
-        <v>189845491</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1">
-        <v>0</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>